<commit_message>
0.2 Finished ETL procedures. Data types WIP
</commit_message>
<xml_diff>
--- a/Table_of_contents.xlsx
+++ b/Table_of_contents.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bluecap\ProgrammingProjects\oracle-sql-cheatsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D399025-9580-43CE-B4B2-6D17108C1B9F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D1B6DFAB-9477-4158-8381-D95518B4870A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" xr2:uid="{87D35531-0D99-475C-B004-19D353972AEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$16</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>WITH</t>
   </si>
@@ -66,9 +69,6 @@
     <t>UPDATE</t>
   </si>
   <si>
-    <t>CREATE TABLE</t>
-  </si>
-  <si>
     <t>Window functions</t>
   </si>
   <si>
@@ -94,6 +94,24 @@
   </si>
   <si>
     <t>Global constants in Oracle SQL</t>
+  </si>
+  <si>
+    <t>CREATE TABLE/VIEW</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>DATA TYPES</t>
+  </si>
+  <si>
+    <t>Data types (ORACLE SQL)</t>
+  </si>
+  <si>
+    <t>INTEGRITY CONSTRAINTS</t>
   </si>
 </sst>
 </file>
@@ -445,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDA787A6-C70B-4D07-803D-506504C08A45}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,135 +474,175 @@
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>20</v>
       </c>
-      <c r="B16" t="s">
-        <v>21</v>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C16" xr:uid="{1DA90599-C9E4-416D-A554-22DCC6BEB089}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
0.3 Finished window functions. Constraints WIP
</commit_message>
<xml_diff>
--- a/Table_of_contents.xlsx
+++ b/Table_of_contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bluecap\ProgrammingProjects\oracle-sql-cheatsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D1B6DFAB-9477-4158-8381-D95518B4870A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F4B37724-7EE6-43FA-8B6C-9A5ABF0CAA44}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" xr2:uid="{87D35531-0D99-475C-B004-19D353972AEA}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$17</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,14 +28,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>WITH</t>
   </si>
   <si>
-    <t>USING</t>
-  </si>
-  <si>
     <t>MATERIALIZE / INLINE / PARALLEL (Hints)</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>INDEXES</t>
   </si>
   <si>
-    <t>PARTITIONS</t>
-  </si>
-  <si>
     <t>WINDOW FUNCTIONS</t>
   </si>
   <si>
@@ -111,7 +105,7 @@
     <t>Data types (ORACLE SQL)</t>
   </si>
   <si>
-    <t>INTEGRITY CONSTRAINTS</t>
+    <t>ADD / DROP CONSTRAINT</t>
   </si>
 </sst>
 </file>
@@ -147,8 +141,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,10 +458,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDA787A6-C70B-4D07-803D-506504C08A45}">
-  <dimension ref="A1:C19"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,29 +472,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -506,7 +508,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -514,7 +516,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -522,7 +524,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -530,7 +532,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -538,7 +540,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -554,7 +559,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -562,87 +570,79 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C16" xr:uid="{1DA90599-C9E4-416D-A554-22DCC6BEB089}"/>
+  <autoFilter ref="A1:C17" xr:uid="{1DA90599-C9E4-416D-A554-22DCC6BEB089}">
+    <filterColumn colId="2">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
0.4 Constraints still WIP. Next step: CHECK Constraint
</commit_message>
<xml_diff>
--- a/Table_of_contents.xlsx
+++ b/Table_of_contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bluecap\ProgrammingProjects\oracle-sql-cheatsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F4B37724-7EE6-43FA-8B6C-9A5ABF0CAA44}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{9F6DBC37-CCBA-489C-9E10-598FD808838B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" xr2:uid="{87D35531-0D99-475C-B004-19D353972AEA}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$18</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>WITH</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>ADD / DROP CONSTRAINT</t>
+  </si>
+  <si>
+    <t>WIP</t>
+  </si>
+  <si>
+    <t>VERIFY, LENGTH, COUNTW, FIND, REPLACE, etc.</t>
   </si>
 </sst>
 </file>
@@ -458,11 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDA787A6-C70B-4D07-803D-506504C08A45}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,7 +486,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -492,7 +497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -529,64 +534,64 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>20</v>
       </c>
       <c r="B13" t="s">
         <v>18</v>
@@ -595,9 +600,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
@@ -606,9 +611,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
@@ -617,31 +622,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>23</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>24</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>25</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>16</v>
       </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C17" xr:uid="{1DA90599-C9E4-416D-A554-22DCC6BEB089}">
-    <filterColumn colId="2">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C18" xr:uid="{1DA90599-C9E4-416D-A554-22DCC6BEB089}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
0.9 Indexes, Variables/Constants (PL/SQL) & Constraints done. FUNCTIONS dictionary WIP.
</commit_message>
<xml_diff>
--- a/Table_of_contents.xlsx
+++ b/Table_of_contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bluecap\ProgrammingProjects\oracle-sql-cheatsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{9F6DBC37-CCBA-489C-9E10-598FD808838B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{82D1A61B-E26A-48EF-AAC9-17F5F06A1B48}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" xr2:uid="{87D35531-0D99-475C-B004-19D353972AEA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>WITH</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>ADD / DROP CONSTRAINT</t>
-  </si>
-  <si>
-    <t>WIP</t>
   </si>
   <si>
     <t>VERIFY, LENGTH, COUNTW, FIND, REPLACE, etc.</t>
@@ -464,10 +461,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDA787A6-C70B-4D07-803D-506504C08A45}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,7 +484,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -497,7 +495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -534,7 +532,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -548,7 +546,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -567,7 +565,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -578,7 +576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -589,7 +587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -600,7 +598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -611,7 +609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -622,7 +620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -633,7 +631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -644,19 +642,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
       </c>
-      <c r="C18" t="s">
-        <v>26</v>
+      <c r="C18">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C18" xr:uid="{1DA90599-C9E4-416D-A554-22DCC6BEB089}"/>
+  <autoFilter ref="A1:C18" xr:uid="{1DA90599-C9E4-416D-A554-22DCC6BEB089}">
+    <filterColumn colId="2">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>